<commit_message>
added register and signin
</commit_message>
<xml_diff>
--- a/bdAppNote.xlsx
+++ b/bdAppNote.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baoying/Desktop/badday/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baoying/Desktop/badmouth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{006DD3BB-5B0D-9148-9C5C-1EB961457820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DEA997-5E9C-644E-8031-B06EA1D9D44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{30133CC2-79ED-7C42-B5A1-9B7C83573DB7}"/>
+    <workbookView xWindow="5160" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{30133CC2-79ED-7C42-B5A1-9B7C83573DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -178,6 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +496,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,13 +520,21 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="10">
+        <v>44664</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5</v>
+      </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="10">
+        <v>44665</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>